<commit_message>
update the example sheet
</commit_message>
<xml_diff>
--- a/public/QuestionsTemplate.xlsx
+++ b/public/QuestionsTemplate.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranza\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\helen\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,34 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>questionType</t>
-  </si>
-  <si>
-    <t>answerSelectionType</t>
-  </si>
-  <si>
-    <t>answers</t>
-  </si>
-  <si>
-    <t>correctAnswer</t>
-  </si>
-  <si>
-    <t>messageForCorrectAnswer</t>
-  </si>
-  <si>
-    <t>messageForIncorrectAnswer</t>
-  </si>
-  <si>
-    <t>explanation</t>
-  </si>
-  <si>
-    <t>point</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>quizTitle</t>
   </si>
@@ -74,19 +48,103 @@
     <t>single</t>
   </si>
   <si>
-    <t>ReactJS is developed by _____?</t>
-  </si>
-  <si>
-    <t>Google Engineers,Facebook Engineers</t>
-  </si>
-  <si>
-    <t>Correct answer. Good job.</t>
-  </si>
-  <si>
-    <t>Incorrect answer. Please try again.</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat.</t>
+    <t>Вопрос 1</t>
+  </si>
+  <si>
+    <t>1 + 1 = …</t>
+  </si>
+  <si>
+    <t>Тип вопроса</t>
+  </si>
+  <si>
+    <t>Выбор ответа</t>
+  </si>
+  <si>
+    <t>Варианты ответов</t>
+  </si>
+  <si>
+    <t>Один,Два,Три</t>
+  </si>
+  <si>
+    <t>Правильный ответ</t>
+  </si>
+  <si>
+    <t>Сообщение для правильного ответа</t>
+  </si>
+  <si>
+    <t>Верный ответ</t>
+  </si>
+  <si>
+    <t>Сообщение для ошибочного ответа</t>
+  </si>
+  <si>
+    <t>Мда кринж…</t>
+  </si>
+  <si>
+    <t>Объяснение решения</t>
+  </si>
+  <si>
+    <t>1 + 1 = 2, потому что …</t>
+  </si>
+  <si>
+    <t>Количество очков</t>
+  </si>
+  <si>
+    <t>Вопрос 2</t>
+  </si>
+  <si>
+    <t>Необходимые знания для управления системами:</t>
+  </si>
+  <si>
+    <t>multiple</t>
+  </si>
+  <si>
+    <t>Поплавок карбюратора,Решение задачи о трех друзьях,Теория управления</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>Сразу видно что умеешь управлять</t>
+  </si>
+  <si>
+    <t>Кто то тут не управленец</t>
+  </si>
+  <si>
+    <t>Нет ну тут все просто - просто не задавай глупых вопросов, всем управленцам нужно знать как работает поплавок карбюратора</t>
+  </si>
+  <si>
+    <t>На листе с вопросами не должно быть ничего кроме двух первых заполненных столбцов</t>
+  </si>
+  <si>
+    <t>Вопросы идут друг за другом без пропусков строк</t>
+  </si>
+  <si>
+    <t>Каждый вопрос занимает ровно 9 строк</t>
+  </si>
+  <si>
+    <t>Атрибут вопроса</t>
+  </si>
+  <si>
+    <t>На текущий момент тип вопроса всегда "text"</t>
+  </si>
+  <si>
+    <t>single если верный ответ 1</t>
+  </si>
+  <si>
+    <t>multiple если верных ответов несколько</t>
+  </si>
+  <si>
+    <t>Варианты ответов перечисляются в одной ячейке через запятую</t>
+  </si>
+  <si>
+    <t>Для одного правильного: Номер правильного ответа (отсчет начиная с единицы)</t>
+  </si>
+  <si>
+    <t>Для нескольких правильных: Номер ответов через запятую, ОБЯЗАТЕЛЬНО после запятых - пробелы (особенность экселя))</t>
+  </si>
+  <si>
+    <t>Каждому вопросу необходимо задать его вес в очках - любое положительное целое число</t>
   </si>
 </sst>
 </file>
@@ -429,191 +487,280 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.36328125" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="B21" s="1">
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>